<commit_message>
new update  for chemstry
</commit_message>
<xml_diff>
--- a/output/phase1/simulation_results_phase1.xlsx
+++ b/output/phase1/simulation_results_phase1.xlsx
@@ -500,13 +500,13 @@
         <v>0.1</v>
       </c>
       <c r="D2" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E2" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F2" t="n">
-        <v>27.65098314606742</v>
+        <v>0.3318117977528089</v>
       </c>
       <c r="G2" t="n">
         <v>207</v>
@@ -532,13 +532,13 @@
         <v>0.2</v>
       </c>
       <c r="D3" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E3" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F3" t="n">
-        <v>55.30196629213484</v>
+        <v>0.6636235955056179</v>
       </c>
       <c r="G3" t="n">
         <v>207</v>
@@ -564,13 +564,13 @@
         <v>0.3</v>
       </c>
       <c r="D4" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E4" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F4" t="n">
-        <v>82.95294943820225</v>
+        <v>0.9954353932584267</v>
       </c>
       <c r="G4" t="n">
         <v>207</v>
@@ -596,13 +596,13 @@
         <v>0.4</v>
       </c>
       <c r="D5" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E5" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F5" t="n">
-        <v>110.6039325842697</v>
+        <v>1.327247191011236</v>
       </c>
       <c r="G5" t="n">
         <v>207</v>
@@ -628,13 +628,13 @@
         <v>0.5</v>
       </c>
       <c r="D6" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E6" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F6" t="n">
-        <v>138.2549157303371</v>
+        <v>1.659058988764045</v>
       </c>
       <c r="G6" t="n">
         <v>207</v>
@@ -660,13 +660,13 @@
         <v>0.6</v>
       </c>
       <c r="D7" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E7" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F7" t="n">
-        <v>165.9058988764045</v>
+        <v>1.990870786516853</v>
       </c>
       <c r="G7" t="n">
         <v>207</v>
@@ -692,13 +692,13 @@
         <v>0.7</v>
       </c>
       <c r="D8" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E8" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F8" t="n">
-        <v>193.5568820224719</v>
+        <v>2.322682584269662</v>
       </c>
       <c r="G8" t="n">
         <v>207</v>
@@ -724,13 +724,13 @@
         <v>0.8</v>
       </c>
       <c r="D9" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E9" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F9" t="n">
-        <v>221.2078651685393</v>
+        <v>2.654494382022472</v>
       </c>
       <c r="G9" t="n">
         <v>207</v>
@@ -756,13 +756,13 @@
         <v>0.9</v>
       </c>
       <c r="D10" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E10" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F10" t="n">
-        <v>248.8588483146067</v>
+        <v>2.98630617977528</v>
       </c>
       <c r="G10" t="n">
         <v>207</v>
@@ -788,13 +788,13 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E11" t="n">
-        <v>2.5</v>
+        <v>0.3</v>
       </c>
       <c r="F11" t="n">
-        <v>276.5098314606742</v>
+        <v>3.318117977528089</v>
       </c>
       <c r="G11" t="n">
         <v>207</v>

</xml_diff>